<commit_message>
fix: incrementati unit test
</commit_message>
<xml_diff>
--- a/house-of-science/core/src/test/resources/com/adiacent/menarini/mhos/core/models/dnnImportLibraryDS.xlsx
+++ b/house-of-science/core/src/test/resources/com/adiacent/menarini/mhos/core/models/dnnImportLibraryDS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francesca.mancini\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F99D927-8A15-4441-8596-1B8C2B66E39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6671C0A9-9CC3-418B-A3FE-2A47F8EF3ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{42D9776E-1A14-43E2-94B2-4398DA74DBA7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Source</t>
   </si>
@@ -62,16 +62,19 @@
     <t>Date articledate</t>
   </si>
   <si>
-    <t>Report</t>
-  </si>
-  <si>
-    <t>ISTAT/ISS</t>
-  </si>
-  <si>
     <t>Impatto Dell’epidemia Covid-19 Sulla Mortalità Totale Della Popolazione Residente Primo Trimestre 2020</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;a class="accordionReadMore" href="https://www.istat.it/it/files/2020/05/Rapporto_Istat_ISS.pdf" target="_blank"&gt;Read More »&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>aroda-vanita-r</t>
+  </si>
+  <si>
+    <t>accademia-dei-lincei</t>
+  </si>
+  <si>
+    <t>articles</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <dimension ref="A1:H137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD35"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,19 +482,19 @@
         <v>43955</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -1577,5 +1580,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>